<commit_message>
v2.2.3; updates and bug fixes to guidance site
</commit_message>
<xml_diff>
--- a/docs/assets/documents/USPTO-Section-508-UI-Mapping.xlsx
+++ b/docs/assets/documents/USPTO-Section-508-UI-Mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20339"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usptogov.sharepoint.com/sites/O3G-PDDDUXBranch/Shared Documents/XD Team - Deliverables/USPTO Design System/508 Research Inclusions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Design System\USPTO-Design-System\dist\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="701" documentId="11_C9A78CC68C934361E875027182C0CD548543469F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{048270EC-106E-4749-A563-AF2B2AE34F5C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F100293-F782-4E61-A008-A9DBFFECA216}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10665" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,8 +27,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -297,7 +297,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1150,18 +1150,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X46" sqref="X46"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="24" thickBot="1">
+    <row r="1" spans="1:31" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="AD1" s="62"/>
       <c r="AE1" s="63"/>
     </row>
-    <row r="2" spans="1:31" ht="24" thickBot="1">
+    <row r="2" spans="1:31" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="64"/>
       <c r="B2" s="65"/>
       <c r="C2" s="65"/>
@@ -1231,7 +1231,7 @@
       <c r="AD2" s="65"/>
       <c r="AE2" s="66"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
@@ -1266,7 +1266,7 @@
       <c r="AD3" s="32"/>
       <c r="AE3" s="33"/>
     </row>
-    <row r="4" spans="1:31" ht="15.75">
+    <row r="4" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -1305,7 +1305,7 @@
       </c>
       <c r="AE4" s="12"/>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>6</v>
       </c>
@@ -1340,7 +1340,7 @@
       <c r="AD5" s="6"/>
       <c r="AE5" s="12"/>
     </row>
-    <row r="6" spans="1:31" ht="15.75">
+    <row r="6" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>7</v>
       </c>
@@ -1383,7 +1383,7 @@
       <c r="AD6" s="6"/>
       <c r="AE6" s="12"/>
     </row>
-    <row r="7" spans="1:31" ht="15.75">
+    <row r="7" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>12</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="15.75">
+    <row r="8" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>19</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
       <c r="B9" s="29"/>
       <c r="C9" s="9"/>
@@ -1518,7 +1518,7 @@
       <c r="AD9" s="9"/>
       <c r="AE9" s="30"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="67" t="s">
         <v>20</v>
       </c>
@@ -1553,7 +1553,7 @@
       <c r="AD10" s="68"/>
       <c r="AE10" s="69"/>
     </row>
-    <row r="11" spans="1:31" ht="15.75">
+    <row r="11" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>21</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="15.75">
+    <row r="12" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>23</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="AD12" s="6"/>
       <c r="AE12" s="12"/>
     </row>
-    <row r="13" spans="1:31" ht="15.75">
+    <row r="13" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>24</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="15.75">
+    <row r="14" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>25</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="15.75">
+    <row r="15" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>28</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="15.75">
+    <row r="16" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>29</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="15.75">
+    <row r="17" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>30</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="15.75">
+    <row r="18" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
         <v>31</v>
       </c>
@@ -1903,7 +1903,7 @@
       <c r="AD18" s="6"/>
       <c r="AE18" s="12"/>
     </row>
-    <row r="19" spans="1:31" ht="15.75">
+    <row r="19" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>32</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="15.75">
+    <row r="20" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>34</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="15.75">
+    <row r="21" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
         <v>35</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="15.75">
+    <row r="22" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
         <v>36</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="15.75">
+    <row r="23" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>37</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="15.75">
+    <row r="24" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
         <v>38</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="15.75">
+    <row r="25" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>39</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="15.75">
+    <row r="26" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
         <v>40</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="15.75">
+    <row r="27" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
         <v>41</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="15.75">
+    <row r="28" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
         <v>42</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="15.75">
+    <row r="29" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
         <v>44</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="15.75">
+    <row r="30" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
         <v>45</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="35"/>
       <c r="B31" s="13"/>
       <c r="C31" s="6"/>
@@ -2503,7 +2503,7 @@
       <c r="AD31" s="6"/>
       <c r="AE31" s="12"/>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="35"/>
       <c r="B32" s="13"/>
       <c r="C32" s="6"/>
@@ -2536,7 +2536,7 @@
       <c r="AD32" s="6"/>
       <c r="AE32" s="12"/>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>46</v>
       </c>
@@ -2571,7 +2571,7 @@
       <c r="AD33" s="6"/>
       <c r="AE33" s="12"/>
     </row>
-    <row r="34" spans="1:31" ht="15.75">
+    <row r="34" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
         <v>47</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="15.75">
+    <row r="35" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>48</v>
       </c>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="AE35" s="12"/>
     </row>
-    <row r="36" spans="1:31" ht="15.75">
+    <row r="36" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
         <v>49</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="15.75">
+    <row r="37" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
         <v>50</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:31" ht="15.75">
+    <row r="38" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
         <v>51</v>
       </c>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="AE38" s="12"/>
     </row>
-    <row r="39" spans="1:31" ht="15.75">
+    <row r="39" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="35" t="s">
         <v>52</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
       <c r="B40" s="13"/>
       <c r="C40" s="6"/>
@@ -2864,7 +2864,7 @@
       <c r="AD40" s="6"/>
       <c r="AE40" s="12"/>
     </row>
-    <row r="41" spans="1:31" ht="15.75">
+    <row r="41" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
         <v>53</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:31" ht="15.75">
+    <row r="42" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
         <v>54</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:31" ht="15.75">
+    <row r="43" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
         <v>56</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:31" ht="15.75">
+    <row r="44" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
         <v>60</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:31" ht="15.75">
+    <row r="45" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
         <v>61</v>
       </c>
@@ -3089,7 +3089,7 @@
       <c r="AD45" s="46"/>
       <c r="AE45" s="12"/>
     </row>
-    <row r="46" spans="1:31" ht="15.75">
+    <row r="46" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
         <v>62</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:31" ht="15.75">
+    <row r="47" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
         <v>63</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
         <v>67</v>
       </c>
@@ -3224,7 +3224,7 @@
       <c r="AD48" s="6"/>
       <c r="AE48" s="12"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="35" t="s">
         <v>68</v>
       </c>
@@ -3259,7 +3259,7 @@
       <c r="AD49" s="6"/>
       <c r="AE49" s="12"/>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="35"/>
       <c r="B50" s="13"/>
       <c r="C50" s="6"/>
@@ -3292,7 +3292,7 @@
       <c r="AD50" s="6"/>
       <c r="AE50" s="12"/>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="37"/>
       <c r="B51" s="13"/>
       <c r="C51" s="6"/>
@@ -3325,7 +3325,7 @@
       <c r="AD51" s="6"/>
       <c r="AE51" s="12"/>
     </row>
-    <row r="52" spans="1:31" ht="15.75" thickBot="1">
+    <row r="52" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="38"/>
       <c r="B52" s="25"/>
       <c r="C52" s="15"/>
@@ -3572,16 +3572,16 @@
   <dimension ref="A1:AJ50"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I30" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="19.5" thickBot="1">
+    <row r="1" spans="1:35" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -3622,7 +3622,7 @@
       <c r="AH1" s="1"/>
       <c r="AI1" s="2"/>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>2</v>
       </c>
@@ -3649,7 +3649,7 @@
       <c r="V2" s="17"/>
       <c r="W2" s="18"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75">
+    <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>3</v>
       </c>
@@ -3690,7 +3690,7 @@
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
     </row>
-    <row r="4" spans="1:35" ht="15.75">
+    <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>6</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
     </row>
-    <row r="5" spans="1:35" ht="15.75">
+    <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>7</v>
       </c>
@@ -3782,7 +3782,7 @@
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
     </row>
-    <row r="6" spans="1:35" ht="15.75">
+    <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>12</v>
       </c>
@@ -3837,7 +3837,7 @@
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
     </row>
-    <row r="7" spans="1:35" ht="15.75">
+    <row r="7" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>19</v>
       </c>
@@ -3886,7 +3886,7 @@
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="35"/>
       <c r="B8" s="11"/>
       <c r="C8" s="10"/>
@@ -3923,7 +3923,7 @@
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
         <v>20</v>
       </c>
@@ -3962,7 +3962,7 @@
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
     </row>
-    <row r="10" spans="1:35" ht="15.75">
+    <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>21</v>
       </c>
@@ -4013,7 +4013,7 @@
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
     </row>
-    <row r="11" spans="1:35" ht="15.75">
+    <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>23</v>
       </c>
@@ -4058,7 +4058,7 @@
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
     </row>
-    <row r="12" spans="1:35" ht="15.75">
+    <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>24</v>
       </c>
@@ -4111,7 +4111,7 @@
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
     </row>
-    <row r="13" spans="1:35" ht="15.75">
+    <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>25</v>
       </c>
@@ -4160,7 +4160,7 @@
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
     </row>
-    <row r="14" spans="1:35" ht="15.75">
+    <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>28</v>
       </c>
@@ -4207,7 +4207,7 @@
       <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
     </row>
-    <row r="15" spans="1:35" ht="15.75">
+    <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>29</v>
       </c>
@@ -4254,7 +4254,7 @@
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
     </row>
-    <row r="16" spans="1:35" ht="15.75">
+    <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>30</v>
       </c>
@@ -4305,7 +4305,7 @@
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
     </row>
-    <row r="17" spans="1:35" ht="15.75">
+    <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>31</v>
       </c>
@@ -4352,7 +4352,7 @@
       <c r="AH17" s="3"/>
       <c r="AI17" s="3"/>
     </row>
-    <row r="18" spans="1:35" ht="15.75">
+    <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
         <v>32</v>
       </c>
@@ -4407,7 +4407,7 @@
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="1:35" ht="15.75">
+    <row r="19" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>34</v>
       </c>
@@ -4460,7 +4460,7 @@
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="1:35" ht="15.75">
+    <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
         <v>35</v>
       </c>
@@ -4513,7 +4513,7 @@
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="1:35" ht="15.75">
+    <row r="21" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
         <v>36</v>
       </c>
@@ -4566,7 +4566,7 @@
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
-    <row r="22" spans="1:35" ht="15.75">
+    <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
         <v>37</v>
       </c>
@@ -4615,7 +4615,7 @@
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
-    <row r="23" spans="1:35" ht="15.75">
+    <row r="23" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>38</v>
       </c>
@@ -4664,7 +4664,7 @@
       <c r="AH23" s="3"/>
       <c r="AI23" s="3"/>
     </row>
-    <row r="24" spans="1:35" ht="15.75">
+    <row r="24" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
         <v>39</v>
       </c>
@@ -4713,7 +4713,7 @@
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="1:35" ht="15.75">
+    <row r="25" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>40</v>
       </c>
@@ -4762,7 +4762,7 @@
       <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
-    <row r="26" spans="1:35" ht="15.75">
+    <row r="26" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
         <v>41</v>
       </c>
@@ -4809,7 +4809,7 @@
       <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
     </row>
-    <row r="27" spans="1:35" ht="15.75">
+    <row r="27" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
         <v>42</v>
       </c>
@@ -4862,7 +4862,7 @@
       <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
     </row>
-    <row r="28" spans="1:35" ht="15.75">
+    <row r="28" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
         <v>44</v>
       </c>
@@ -4913,7 +4913,7 @@
       <c r="AH28" s="3"/>
       <c r="AI28" s="3"/>
     </row>
-    <row r="29" spans="1:35" ht="15.75">
+    <row r="29" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
         <v>45</v>
       </c>
@@ -4962,7 +4962,7 @@
       <c r="AH29" s="3"/>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="35"/>
       <c r="B30" s="11"/>
       <c r="C30" s="10"/>
@@ -4999,7 +4999,7 @@
       <c r="AH30" s="3"/>
       <c r="AI30" s="3"/>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="35"/>
       <c r="B31" s="11"/>
       <c r="C31" s="10"/>
@@ -5036,7 +5036,7 @@
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
         <v>46</v>
       </c>
@@ -5075,7 +5075,7 @@
       <c r="AH32" s="3"/>
       <c r="AI32" s="3"/>
     </row>
-    <row r="33" spans="1:36" ht="15.75">
+    <row r="33" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>47</v>
       </c>
@@ -5126,7 +5126,7 @@
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
     </row>
-    <row r="34" spans="1:36" ht="15.75">
+    <row r="34" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
         <v>48</v>
       </c>
@@ -5169,7 +5169,7 @@
       <c r="AH34" s="3"/>
       <c r="AI34" s="3"/>
     </row>
-    <row r="35" spans="1:36" ht="15.75">
+    <row r="35" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>49</v>
       </c>
@@ -5214,7 +5214,7 @@
       <c r="AH35" s="3"/>
       <c r="AI35" s="3"/>
     </row>
-    <row r="36" spans="1:36" ht="15.75">
+    <row r="36" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
         <v>50</v>
       </c>
@@ -5267,7 +5267,7 @@
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
     </row>
-    <row r="37" spans="1:36" ht="15.75">
+    <row r="37" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
         <v>51</v>
       </c>
@@ -5308,7 +5308,7 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
     </row>
-    <row r="38" spans="1:36" ht="15.75">
+    <row r="38" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
         <v>52</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="AI38" s="3"/>
       <c r="AJ38" s="3"/>
     </row>
-    <row r="39" spans="1:36">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
       <c r="B39" s="11"/>
       <c r="C39" s="10"/>
@@ -5398,7 +5398,7 @@
       <c r="AI39" s="3"/>
       <c r="AJ39" s="3"/>
     </row>
-    <row r="40" spans="1:36" ht="15.75">
+    <row r="40" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>53</v>
       </c>
@@ -5454,7 +5454,7 @@
       <c r="AI40" s="3"/>
       <c r="AJ40" s="3"/>
     </row>
-    <row r="41" spans="1:36" ht="15.75">
+    <row r="41" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
         <v>54</v>
       </c>
@@ -5491,7 +5491,7 @@
       <c r="AI41" s="3"/>
       <c r="AJ41" s="3"/>
     </row>
-    <row r="42" spans="1:36" ht="15.75">
+    <row r="42" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
         <v>56</v>
       </c>
@@ -5525,7 +5525,7 @@
       <c r="AI42" s="3"/>
       <c r="AJ42" s="3"/>
     </row>
-    <row r="43" spans="1:36" ht="15.75">
+    <row r="43" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
         <v>60</v>
       </c>
@@ -5565,7 +5565,7 @@
       <c r="AI43" s="3"/>
       <c r="AJ43" s="3"/>
     </row>
-    <row r="44" spans="1:36" ht="15.75">
+    <row r="44" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
         <v>61</v>
       </c>
@@ -5605,7 +5605,7 @@
       <c r="AI44" s="3"/>
       <c r="AJ44" s="3"/>
     </row>
-    <row r="45" spans="1:36" ht="15.75">
+    <row r="45" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
         <v>62</v>
       </c>
@@ -5649,7 +5649,7 @@
       <c r="AI45" s="3"/>
       <c r="AJ45" s="3"/>
     </row>
-    <row r="46" spans="1:36" ht="15.75">
+    <row r="46" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
         <v>63</v>
       </c>
@@ -5698,7 +5698,7 @@
       <c r="AI46" s="3"/>
       <c r="AJ46" s="3"/>
     </row>
-    <row r="47" spans="1:36" ht="15.75">
+    <row r="47" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
         <v>67</v>
       </c>
@@ -5737,7 +5737,7 @@
       <c r="AI47" s="3"/>
       <c r="AJ47" s="3"/>
     </row>
-    <row r="48" spans="1:36" ht="15.75">
+    <row r="48" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
         <v>68</v>
       </c>
@@ -5776,7 +5776,7 @@
       <c r="AI48" s="3"/>
       <c r="AJ48" s="3"/>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="44"/>
       <c r="B49" s="11"/>
       <c r="C49" s="10"/>
@@ -5805,7 +5805,7 @@
       <c r="AI49" s="3"/>
       <c r="AJ49" s="3"/>
     </row>
-    <row r="50" spans="1:36" ht="15.75" thickBot="1">
+    <row r="50" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="45"/>
       <c r="B50" s="14"/>
       <c r="C50" s="21"/>
@@ -6284,13 +6284,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B746C95-6940-4D19-B5A0-4E7FE1EDB40D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B746C95-6940-4D19-B5A0-4E7FE1EDB40D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD19F61B-94FF-4742-BFAF-E7496C7B697C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD19F61B-94FF-4742-BFAF-E7496C7B697C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="695f8306-c33c-43b8-8b16-647349f48b9e"/>
+    <ds:schemaRef ds:uri="56d5abc5-b3cf-410f-a593-8de3d671d3c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D0B100-2606-4EAB-9A41-AD1DF051AE74}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D0B100-2606-4EAB-9A41-AD1DF051AE74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="56d5abc5-b3cf-410f-a593-8de3d671d3c9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="695f8306-c33c-43b8-8b16-647349f48b9e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>